<commit_message>
import excel sudah sesuai
</commit_message>
<xml_diff>
--- a/assets/file/Template_Excel.xlsx
+++ b/assets/file/Template_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lukman\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633E11D2-F458-4D1B-83CB-1D46F6E87546}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1ED9C3-585D-4808-ABD1-0A538D0362C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7188" yWindow="2292" windowWidth="15336" windowHeight="8016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>JENIS KENDARAAN</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>NOPOL</t>
+  </si>
+  <si>
+    <t>KM TERBARU</t>
+  </si>
+  <si>
+    <t>KM SERVIS</t>
   </si>
 </sst>
 </file>
@@ -62,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -137,7 +143,9 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -153,7 +161,7 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -444,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,10 +470,12 @@
     <col min="8" max="8" width="18.44140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="13" style="1" customWidth="1"/>
     <col min="10" max="10" width="25.33203125" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="3"/>
+    <col min="11" max="11" width="12.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>9</v>
       </c>
@@ -493,8 +503,14 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>